<commit_message>
Update Cardinality Smoker Stats nonSmoker, New Approach for Classifiacation
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cde-tobacco-smoking-status.xlsx
+++ b/output/StructureDefinition-cde-tobacco-smoking-status.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-06T11:09:37+01:00</t>
+    <t>2023-03-06T11:31:12+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -114,7 +114,7 @@
     <t>Base Definition</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/StructureDefinition/Observation</t>
+    <t>http://somewhere.org/fhir/uv/myig/StructureDefinition/cls-snomed-finding-of-tobacco-use-and-exposure</t>
   </si>
   <si>
     <t>Abstract</t>
@@ -19088,10 +19088,10 @@
         <v>80</v>
       </c>
       <c r="G136" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H136" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I136" t="s" s="2">
         <v>82</v>
@@ -19173,7 +19173,7 @@
         <v>104</v>
       </c>
       <c r="AJ136" t="s" s="2">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="AK136" t="s" s="2">
         <v>82</v>
@@ -21756,10 +21756,10 @@
         <v>80</v>
       </c>
       <c r="G158" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H158" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I158" t="s" s="2">
         <v>82</v>
@@ -21841,7 +21841,7 @@
         <v>104</v>
       </c>
       <c r="AJ158" t="s" s="2">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="AK158" t="s" s="2">
         <v>82</v>
@@ -24424,10 +24424,10 @@
         <v>80</v>
       </c>
       <c r="G180" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H180" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I180" t="s" s="2">
         <v>82</v>
@@ -24509,7 +24509,7 @@
         <v>104</v>
       </c>
       <c r="AJ180" t="s" s="2">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="AK180" t="s" s="2">
         <v>82</v>
@@ -27092,10 +27092,10 @@
         <v>80</v>
       </c>
       <c r="G202" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H202" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I202" t="s" s="2">
         <v>82</v>
@@ -27177,7 +27177,7 @@
         <v>104</v>
       </c>
       <c r="AJ202" t="s" s="2">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="AK202" t="s" s="2">
         <v>82</v>
@@ -28413,13 +28413,13 @@
       </c>
       <c r="E213" s="2"/>
       <c r="F213" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G213" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H213" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I213" t="s" s="2">
         <v>82</v>
@@ -28661,7 +28661,7 @@
         <v>92</v>
       </c>
       <c r="H215" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I215" t="s" s="2">
         <v>82</v>

</xml_diff>